<commit_message>
v2: specs and testing cleanup
</commit_message>
<xml_diff>
--- a/v2/documentation/Specs_v2.xlsx
+++ b/v2/documentation/Specs_v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>If both distances are the same, output first ID</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>STATUS</t>
+  </si>
+  <si>
+    <t>TESTING</t>
   </si>
 </sst>
 </file>
@@ -756,7 +759,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +987,9 @@
       <c r="E15" s="24">
         <v>0.5</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -1010,7 +1015,9 @@
       <c r="E17" s="30">
         <v>0.5</v>
       </c>
-      <c r="F17" s="31"/>
+      <c r="F17" s="31" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>

</xml_diff>